<commit_message>
added bloom perf analysis
</commit_message>
<xml_diff>
--- a/docs/perf.xlsx
+++ b/docs/perf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jian Ru\Documents\CIS565\final_project\laugh_engine\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jian Ru\Documents\Personal_Projects\Laugh_Engine\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Boom Box</t>
+  </si>
+  <si>
+    <t>Corset</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Lantern</t>
+  </si>
+  <si>
+    <t>Microphone</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1642,6 +1671,617 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Bloom Optimization</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>After optimization</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>Avocado</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Fish</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Boom Box</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Corset</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Helmet</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Lantern</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Microphone</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>Telephone</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D71-4957-9FBB-2D137FF492BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Before optimization</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="8"/>
+              <c:pt idx="0">
+                <c:v>Avocado</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Fish</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Boom Box</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Corset</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Helmet</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Lantern</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Microphone</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>Telephone</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D71-4957-9FBB-2D137FF492BE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="330184952"/>
+        <c:axId val="330184624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="330184952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330184624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="330184624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frame Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="330184952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1762,6 +2402,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="234">
   <cs:axisTitle>
@@ -3278,6 +3958,511 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3358,16 +4543,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3387,6 +4572,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5D47ECF-FA2F-4254-957B-9B096D7DC745}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3692,15 +4913,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B9"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>222.78</v>
       </c>
@@ -3723,7 +4944,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>15.59</v>
       </c>
@@ -3740,7 +4961,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2.52</v>
       </c>
@@ -3748,7 +4969,7 @@
         <v>19.36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2.46</v>
       </c>
@@ -3756,6 +4977,84 @@
         <v>19.04</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2.69</v>
+      </c>
+      <c r="B13">
+        <v>2.82</v>
+      </c>
+      <c r="C13">
+        <v>3.23</v>
+      </c>
+      <c r="D13">
+        <v>2.75</v>
+      </c>
+      <c r="E13">
+        <v>4.05</v>
+      </c>
+      <c r="F13">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G13">
+        <v>3.03</v>
+      </c>
+      <c r="H13">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3.51</v>
+      </c>
+      <c r="B14">
+        <v>3.68</v>
+      </c>
+      <c r="C14">
+        <v>4.09</v>
+      </c>
+      <c r="D14">
+        <v>3.59</v>
+      </c>
+      <c r="E14">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="F14">
+        <v>3.39</v>
+      </c>
+      <c r="G14">
+        <v>3.91</v>
+      </c>
+      <c r="H14">
+        <v>3.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>